<commit_message>
se modificó la carga del script de los Forms de PC.
</commit_message>
<xml_diff>
--- a/CardaData/DataSource - CargaFormsPC.xlsx
+++ b/CardaData/DataSource - CargaFormsPC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\CardaData\DataSource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\CardaData\CardaData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06D3D179-CC2E-49E9-8291-651B44527EAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{651E0106-05CA-41A0-AC40-C6A76F4A9552}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="24">
   <si>
     <t>Usuario</t>
   </si>
@@ -51,16 +51,52 @@
     <t>https://suragwqa2.segurossura.com.ar/pc/PolicyCenter.do</t>
   </si>
   <si>
-    <t>ssurgwsoadev4.opc.oracleoutsourcing.com</t>
-  </si>
-  <si>
-    <t>https://ssurgwsoadev4.opc.oracleoutsourcing.com/pc/PolicyCenter.do</t>
-  </si>
-  <si>
     <t>ssurgwsoadev4-oci.opc.oracleoutsourcing.com</t>
   </si>
   <si>
     <t>https://ssurgwsoadev4-oci.opc.oracleoutsourcing.com/pc/PolicyCenter.do</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>NombreArchivo</t>
+  </si>
+  <si>
+    <t>ASISTMED.xml</t>
+  </si>
+  <si>
+    <t>CACGCCPA_AP_01.xml</t>
+  </si>
+  <si>
+    <t>CRAAP.xml</t>
+  </si>
+  <si>
+    <t>de4412.xml</t>
+  </si>
+  <si>
+    <t>IEPHO.xml</t>
+  </si>
+  <si>
+    <t>policy forms SURA.xml</t>
+  </si>
+  <si>
+    <t>TFS38586_SO_RC_4_1.xml</t>
+  </si>
+  <si>
+    <t>tfs42429_Form_CECSMAP.xml</t>
+  </si>
+  <si>
+    <t>TFS42483_forms_CAC_CC_18_1.xml</t>
+  </si>
+  <si>
+    <t>TFS43183 - ASISTMED.xml</t>
+  </si>
+  <si>
+    <t>TFS45166_TREEHO_2344.xml</t>
+  </si>
+  <si>
+    <t>TFS46199_policy forms.xml</t>
   </si>
 </sst>
 </file>
@@ -396,82 +432,538 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A13" sqref="A13:A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="58" customWidth="1"/>
-    <col min="2" max="2" width="60" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="58" customWidth="1"/>
+    <col min="3" max="3" width="60" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
+    <col min="6" max="6" width="32.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
+      <c r="B12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" t="s">
+        <v>5</v>
+      </c>
+      <c r="F23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" t="s">
+        <v>5</v>
+      </c>
+      <c r="F24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" t="s">
+        <v>5</v>
+      </c>
+      <c r="F25" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{9A97D6B9-B8FF-4E1E-8511-84B4E34F4F57}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{FB7616B4-D05B-4941-BECC-4C85F482A38C}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{63B0416F-942C-43EE-BC47-D521EA103788}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{14C90322-CF21-4B5B-BDE0-9EF5DC08288E}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{9141B99B-43C1-4179-9A5E-62AF408CC7E1}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{8AC5792E-3753-431D-87C5-A2107FF4AA30}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{0A43FB6E-D314-4919-A92F-04484F58CE6D}"/>
+    <hyperlink ref="C8" r:id="rId7" xr:uid="{415FB8A2-06E8-41BD-88C5-F36FDBF3E95C}"/>
+    <hyperlink ref="C9" r:id="rId8" xr:uid="{2D121E87-0638-487F-B241-B54D0F4F1E62}"/>
+    <hyperlink ref="C10" r:id="rId9" xr:uid="{CF259F38-4139-4FB0-9816-4E4158A38FFB}"/>
+    <hyperlink ref="C11" r:id="rId10" xr:uid="{8DE9F0AB-73E4-401D-A462-0E60D8E18213}"/>
+    <hyperlink ref="C12" r:id="rId11" xr:uid="{2148CCF6-1DBC-47B8-8117-9C0F86D4DFC6}"/>
+    <hyperlink ref="C13" r:id="rId12" xr:uid="{40F3A1BD-36BC-466B-9FC3-F206108CB119}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>